<commit_message>
added GUI files, and menu when exporting to spreadsheet
</commit_message>
<xml_diff>
--- a/main/other/Copy_of_updated_Hardware3.xlsx
+++ b/main/other/Copy_of_updated_Hardware3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mackayp\moordesign\main\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E87ABDE-0F01-450C-BB7C-D5CEB75D75ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1060DF-A218-49DE-884D-DA1901CBED1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13068" yWindow="-2880" windowWidth="13176" windowHeight="22656" xr2:uid="{4E9EA262-9DA5-4196-B65F-CFA2DC6E9F4D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4E9EA262-9DA5-4196-B65F-CFA2DC6E9F4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -946,8 +946,8 @@
   <dimension ref="A1:I93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H40" sqref="A40:H40"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>